<commit_message>
Add DEMO_02 Edge Project
</commit_message>
<xml_diff>
--- a/Master/DEMO/Przechwytywanie Danych/DEMO_02/File Excel/challenge.xlsx
+++ b/Master/DEMO/Przechwytywanie Danych/DEMO_02/File Excel/challenge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kudzi\source\repos\UiPath-Demo\UiPath-Demo\Master\DEMO\Przechwytywanie Danych\DEMO_02\File Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7FA2E4-74BF-4480-B10E-1CCA49E6F75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365EEEA1-CBD2-4160-A37B-BE96572F4896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="3315" windowWidth="34530" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="4260" windowWidth="34530" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1189,12 +1189,12 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.75" bestFit="1" customWidth="1"/>

</xml_diff>